<commit_message>
Leitura dos dados do site
</commit_message>
<xml_diff>
--- a/data/Ações para consulta.xlsx
+++ b/data/Ações para consulta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paulo\Desktop\Projetos\Fundamentus\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526D7ED3-6463-4706-9EAA-D0BB06866398}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7605635-D699-4F0A-8E95-5D90A1D5806A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27735" yWindow="660" windowWidth="27855" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -420,10 +420,13 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B2" sqref="B2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">

</xml_diff>